<commit_message>
fixed a bug in the compound_featurizer.py when a structure has multiple non_transition metals along with other demo notebooks and README.md updates
</commit_message>
<xml_diff>
--- a/data/torrance_tables/torrance_tabulated.xlsx
+++ b/data/torrance_tables/torrance_tabulated.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonrpw/PycharmProjects/mit_model_code/data/torrance_tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9421FE1E-67CD-3344-9FC0-6C0E25015EB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28FECC6C-C51F-614D-A07B-0CA1ACB59E4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="19160" windowHeight="20020" xr2:uid="{A66ED206-FB3C-6347-8C90-7D424F3668D5}"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="19160" windowHeight="19920" activeTab="1" xr2:uid="{A66ED206-FB3C-6347-8C90-7D424F3668D5}"/>
   </bookViews>
   <sheets>
     <sheet name="table_2" sheetId="1" r:id="rId1"/>
@@ -261,9 +261,6 @@
     <t>r62</t>
   </si>
   <si>
-    <t xml:space="preserve">Ce2O3 </t>
-  </si>
-  <si>
     <t>r63</t>
   </si>
   <si>
@@ -477,9 +474,6 @@
     <t>b-Mn2O3</t>
   </si>
   <si>
-    <t xml:space="preserve">Ia-3 </t>
-  </si>
-  <si>
     <t>LaMnO3</t>
   </si>
   <si>
@@ -706,6 +700,12 @@
   </si>
   <si>
     <t>In2O3</t>
+  </si>
+  <si>
+    <t>Ia-3</t>
+  </si>
+  <si>
+    <t>Ce2O3</t>
   </si>
 </sst>
 </file>
@@ -1069,65 +1069,65 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FF9F47A-8CB9-0E48-BCB1-654019AE6A49}">
   <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" t="s">
         <v>111</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>112</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>113</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>114</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>115</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>116</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>117</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
+        <v>220</v>
+      </c>
+      <c r="J1" t="s">
         <v>118</v>
       </c>
-      <c r="I1" t="s">
-        <v>222</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>119</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>120</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>121</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>122</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>123</v>
       </c>
-      <c r="O1" t="s">
-        <v>124</v>
-      </c>
       <c r="P1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -1136,7 +1136,7 @@
         <v>225</v>
       </c>
       <c r="D2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E2">
         <v>2.1059999999999999</v>
@@ -1177,7 +1177,7 @@
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -1186,7 +1186,7 @@
         <v>167</v>
       </c>
       <c r="D3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E3">
         <v>1.8560000000000001</v>
@@ -1227,16 +1227,16 @@
     </row>
     <row r="4" spans="1:16">
       <c r="A4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C4">
         <v>152</v>
       </c>
       <c r="D4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E4">
         <v>1.609</v>
@@ -1277,7 +1277,7 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
@@ -1286,7 +1286,7 @@
         <v>225</v>
       </c>
       <c r="D5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E5">
         <v>2.399</v>
@@ -1327,16 +1327,16 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C6">
         <v>206</v>
       </c>
       <c r="D6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E6">
         <v>2.121</v>
@@ -1377,16 +1377,16 @@
     </row>
     <row r="7" spans="1:16">
       <c r="A7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" t="s">
         <v>99</v>
-      </c>
-      <c r="B7" t="s">
-        <v>100</v>
       </c>
       <c r="C7">
         <v>136</v>
       </c>
       <c r="D7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E7">
         <v>1.946</v>
@@ -1427,16 +1427,16 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C8">
         <v>201</v>
       </c>
       <c r="D8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E8">
         <v>1.849</v>
@@ -1477,16 +1477,16 @@
     </row>
     <row r="9" spans="1:16">
       <c r="A9" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B9" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C9">
         <v>186</v>
       </c>
       <c r="D9" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E9">
         <v>1.9810000000000001</v>
@@ -1527,16 +1527,16 @@
     </row>
     <row r="10" spans="1:16">
       <c r="A10" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C10">
         <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E10">
         <v>1.94</v>
@@ -1577,7 +1577,7 @@
     </row>
     <row r="11" spans="1:16">
       <c r="A11" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B11" t="s">
         <v>0</v>
@@ -1586,7 +1586,7 @@
         <v>225</v>
       </c>
       <c r="D11" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E11">
         <v>2.5720000000000001</v>
@@ -1627,16 +1627,16 @@
     </row>
     <row r="12" spans="1:16">
       <c r="A12" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C12">
         <v>206</v>
       </c>
       <c r="D12" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E12">
         <v>2.2730000000000001</v>
@@ -1677,7 +1677,7 @@
     </row>
     <row r="13" spans="1:16">
       <c r="A13" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B13" t="s">
         <v>48</v>
@@ -1686,7 +1686,7 @@
         <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E13">
         <v>2.1579999999999999</v>
@@ -1727,7 +1727,7 @@
     </row>
     <row r="14" spans="1:16">
       <c r="A14" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B14" t="s">
         <v>0</v>
@@ -1736,7 +1736,7 @@
         <v>225</v>
       </c>
       <c r="D14" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E14">
         <v>2.3479999999999999</v>
@@ -1777,7 +1777,7 @@
     </row>
     <row r="15" spans="1:16">
       <c r="A15" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B15" t="s">
         <v>2</v>
@@ -1786,7 +1786,7 @@
         <v>167</v>
       </c>
       <c r="D15" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E15">
         <v>2.1869999999999998</v>
@@ -1830,13 +1830,13 @@
         <v>64</v>
       </c>
       <c r="B16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C16">
         <v>136</v>
       </c>
       <c r="D16" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E16">
         <v>2.052</v>
@@ -1877,7 +1877,7 @@
     </row>
     <row r="17" spans="1:16">
       <c r="A17" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B17" t="s">
         <v>0</v>
@@ -1886,7 +1886,7 @@
         <v>225</v>
       </c>
       <c r="D17" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E17">
         <v>2.762</v>
@@ -1927,7 +1927,7 @@
     </row>
     <row r="18" spans="1:16">
       <c r="A18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B18" t="s">
         <v>0</v>
@@ -1936,7 +1936,7 @@
         <v>225</v>
       </c>
       <c r="D18" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E18">
         <v>2.343</v>
@@ -1987,65 +1987,65 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1942F83F-7006-9F48-AB36-DD78CEED56C3}">
   <dimension ref="A1:P77"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" t="s">
         <v>111</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>112</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>113</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>114</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>115</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>116</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>117</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
+        <v>220</v>
+      </c>
+      <c r="J1" t="s">
         <v>118</v>
       </c>
-      <c r="I1" t="s">
-        <v>222</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>119</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>120</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>121</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>122</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>123</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>124</v>
-      </c>
-      <c r="P1" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -2054,7 +2054,7 @@
         <v>225</v>
       </c>
       <c r="D2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E2">
         <v>2.0910000000000002</v>
@@ -2095,7 +2095,7 @@
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -2145,7 +2145,7 @@
     </row>
     <row r="4" spans="1:16">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -2195,10 +2195,10 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" t="s">
         <v>99</v>
-      </c>
-      <c r="B5" t="s">
-        <v>100</v>
       </c>
       <c r="C5">
         <v>136</v>
@@ -2245,7 +2245,7 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
@@ -2295,10 +2295,10 @@
     </row>
     <row r="7" spans="1:16">
       <c r="A7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C7">
         <v>139</v>
@@ -2345,7 +2345,7 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B8" t="s">
         <v>0</v>
@@ -2395,7 +2395,7 @@
     </row>
     <row r="9" spans="1:16">
       <c r="A9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B9" t="s">
         <v>2</v>
@@ -2445,7 +2445,7 @@
     </row>
     <row r="10" spans="1:16">
       <c r="A10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
@@ -2495,16 +2495,16 @@
     </row>
     <row r="11" spans="1:16">
       <c r="A11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C11">
         <v>139</v>
       </c>
       <c r="D11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E11">
         <v>1.9350000000000001</v>
@@ -2545,7 +2545,7 @@
     </row>
     <row r="12" spans="1:16">
       <c r="A12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B12" t="s">
         <v>48</v>
@@ -2554,7 +2554,7 @@
         <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E12">
         <v>1.9339999999999999</v>
@@ -2604,7 +2604,7 @@
         <v>221</v>
       </c>
       <c r="D13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E13">
         <v>1.919</v>
@@ -2645,16 +2645,16 @@
     </row>
     <row r="14" spans="1:16">
       <c r="A14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C14">
         <v>139</v>
       </c>
       <c r="D14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E14">
         <v>1.917</v>
@@ -2695,7 +2695,7 @@
     </row>
     <row r="15" spans="1:16">
       <c r="A15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B15" t="s">
         <v>2</v>
@@ -2704,7 +2704,7 @@
         <v>167</v>
       </c>
       <c r="D15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E15">
         <v>1.9630000000000001</v>
@@ -2745,7 +2745,7 @@
     </row>
     <row r="16" spans="1:16">
       <c r="A16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B16" t="s">
         <v>5</v>
@@ -2754,7 +2754,7 @@
         <v>62</v>
       </c>
       <c r="D16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E16">
         <v>1.97</v>
@@ -2795,16 +2795,16 @@
     </row>
     <row r="17" spans="1:16">
       <c r="A17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C17">
         <v>139</v>
       </c>
       <c r="D17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E17">
         <v>1.92</v>
@@ -2836,16 +2836,16 @@
     </row>
     <row r="18" spans="1:16">
       <c r="A18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C18">
         <v>136</v>
       </c>
       <c r="D18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E18">
         <v>1.8819999999999999</v>
@@ -2886,7 +2886,7 @@
     </row>
     <row r="19" spans="1:16">
       <c r="A19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B19" t="s">
         <v>15</v>
@@ -2895,7 +2895,7 @@
         <v>221</v>
       </c>
       <c r="D19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E19">
         <v>1.909</v>
@@ -2945,7 +2945,7 @@
         <v>225</v>
       </c>
       <c r="D20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E20">
         <v>2.222</v>
@@ -2986,10 +2986,10 @@
     </row>
     <row r="21" spans="1:16">
       <c r="A21" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B21" t="s">
-        <v>147</v>
+        <v>222</v>
       </c>
       <c r="C21">
         <v>206</v>
@@ -3036,7 +3036,7 @@
     </row>
     <row r="22" spans="1:16">
       <c r="A22" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B22" t="s">
         <v>2</v>
@@ -3086,10 +3086,10 @@
     </row>
     <row r="23" spans="1:16">
       <c r="A23" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C23">
         <v>139</v>
@@ -3127,16 +3127,16 @@
     </row>
     <row r="24" spans="1:16">
       <c r="A24" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B24" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C24">
         <v>136</v>
       </c>
       <c r="D24" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E24">
         <v>1.887</v>
@@ -3177,7 +3177,7 @@
     </row>
     <row r="25" spans="1:16">
       <c r="A25" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B25" t="s">
         <v>15</v>
@@ -3227,16 +3227,16 @@
     </row>
     <row r="26" spans="1:16">
       <c r="A26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B26" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C26">
         <v>139</v>
       </c>
       <c r="D26" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E26">
         <v>1.8939999999999999</v>
@@ -3277,7 +3277,7 @@
     </row>
     <row r="27" spans="1:16">
       <c r="A27" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B27" t="s">
         <v>0</v>
@@ -3327,7 +3327,7 @@
     </row>
     <row r="28" spans="1:16">
       <c r="A28" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B28" t="s">
         <v>2</v>
@@ -3377,7 +3377,7 @@
     </row>
     <row r="29" spans="1:16">
       <c r="A29" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B29" t="s">
         <v>5</v>
@@ -3386,7 +3386,7 @@
         <v>62</v>
       </c>
       <c r="D29" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E29">
         <v>2.0059999999999998</v>
@@ -3427,16 +3427,16 @@
     </row>
     <row r="30" spans="1:16">
       <c r="A30" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B30" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C30">
         <v>139</v>
       </c>
       <c r="D30" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E30">
         <v>1.94</v>
@@ -3477,7 +3477,7 @@
     </row>
     <row r="31" spans="1:16">
       <c r="A31" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B31" t="s">
         <v>15</v>
@@ -3486,7 +3486,7 @@
         <v>221</v>
       </c>
       <c r="D31" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E31">
         <v>1.9350000000000001</v>
@@ -3536,7 +3536,7 @@
         <v>225</v>
       </c>
       <c r="D32" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E32">
         <v>2.133</v>
@@ -3577,7 +3577,7 @@
     </row>
     <row r="33" spans="1:16">
       <c r="A33" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B33" t="s">
         <v>25</v>
@@ -3627,7 +3627,7 @@
     </row>
     <row r="34" spans="1:16">
       <c r="A34" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B34" t="s">
         <v>2</v>
@@ -3636,7 +3636,7 @@
         <v>167</v>
       </c>
       <c r="D34" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E34">
         <v>1.9319999999999999</v>
@@ -3677,10 +3677,10 @@
     </row>
     <row r="35" spans="1:16">
       <c r="A35" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B35" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C35">
         <v>139</v>
@@ -3727,7 +3727,7 @@
     </row>
     <row r="36" spans="1:16">
       <c r="A36" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B36" t="s">
         <v>15</v>
@@ -3736,7 +3736,7 @@
         <v>221</v>
       </c>
       <c r="D36" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E36">
         <v>1.931</v>
@@ -3830,7 +3830,7 @@
         <v>30</v>
       </c>
       <c r="B38" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C38">
         <v>139</v>
@@ -3877,7 +3877,7 @@
     </row>
     <row r="39" spans="1:16">
       <c r="A39" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B39" t="s">
         <v>2</v>
@@ -3927,10 +3927,10 @@
     </row>
     <row r="40" spans="1:16">
       <c r="A40" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B40" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C40">
         <v>139</v>
@@ -4077,7 +4077,7 @@
     </row>
     <row r="43" spans="1:16">
       <c r="A43" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B43" t="s">
         <v>2</v>
@@ -4130,7 +4130,7 @@
         <v>41</v>
       </c>
       <c r="B44" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C44">
         <v>139</v>
@@ -4230,7 +4230,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C46">
         <v>88</v>
@@ -4380,7 +4380,7 @@
         <v>52</v>
       </c>
       <c r="B49" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C49">
         <v>139</v>
@@ -4427,7 +4427,7 @@
     </row>
     <row r="50" spans="1:16">
       <c r="A50" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B50" t="s">
         <v>15</v>
@@ -4477,10 +4477,10 @@
     </row>
     <row r="51" spans="1:16">
       <c r="A51" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B51" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C51">
         <v>136</v>
@@ -4527,7 +4527,7 @@
     </row>
     <row r="52" spans="1:16">
       <c r="A52" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B52" t="s">
         <v>15</v>
@@ -4577,10 +4577,10 @@
     </row>
     <row r="53" spans="1:16">
       <c r="A53" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B53" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C53">
         <v>139</v>
@@ -4627,7 +4627,7 @@
     </row>
     <row r="54" spans="1:16">
       <c r="A54" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B54" t="s">
         <v>2</v>
@@ -4668,7 +4668,7 @@
     </row>
     <row r="55" spans="1:16">
       <c r="A55" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B55" t="s">
         <v>15</v>
@@ -4718,10 +4718,10 @@
     </row>
     <row r="56" spans="1:16">
       <c r="A56" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B56" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C56">
         <v>136</v>
@@ -4821,7 +4821,7 @@
         <v>64</v>
       </c>
       <c r="B58" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C58">
         <v>136</v>
@@ -4868,7 +4868,7 @@
     </row>
     <row r="59" spans="1:16">
       <c r="A59" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B59" t="s">
         <v>15</v>
@@ -4921,7 +4921,7 @@
         <v>67</v>
       </c>
       <c r="B60" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C60">
         <v>139</v>
@@ -5021,7 +5021,7 @@
         <v>71</v>
       </c>
       <c r="B62" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C62">
         <v>164</v>
@@ -5118,16 +5118,16 @@
     </row>
     <row r="64" spans="1:16">
       <c r="A64" t="s">
-        <v>75</v>
+        <v>223</v>
       </c>
       <c r="B64" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C64">
         <v>164</v>
       </c>
       <c r="D64" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E64">
         <v>2.3420000000000001</v>
@@ -5168,7 +5168,7 @@
     </row>
     <row r="65" spans="1:16">
       <c r="A65" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B65" t="s">
         <v>0</v>
@@ -5177,7 +5177,7 @@
         <v>225</v>
       </c>
       <c r="D65" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E65">
         <v>2.343</v>
@@ -5218,7 +5218,7 @@
     </row>
     <row r="66" spans="1:16">
       <c r="A66" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B66" t="s">
         <v>15</v>
@@ -5227,7 +5227,7 @@
         <v>221</v>
       </c>
       <c r="D66" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E66">
         <v>2.1459999999999999</v>
@@ -5268,7 +5268,7 @@
     </row>
     <row r="67" spans="1:16">
       <c r="A67" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B67" t="s">
         <v>0</v>
@@ -5277,7 +5277,7 @@
         <v>225</v>
       </c>
       <c r="D67" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E67">
         <v>2.516</v>
@@ -5318,16 +5318,16 @@
     </row>
     <row r="68" spans="1:16">
       <c r="A68" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B68" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C68">
         <v>164</v>
       </c>
       <c r="D68" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E68">
         <v>2.3450000000000002</v>
@@ -5368,7 +5368,7 @@
     </row>
     <row r="69" spans="1:16">
       <c r="A69" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B69" t="s">
         <v>0</v>
@@ -5377,7 +5377,7 @@
         <v>225</v>
       </c>
       <c r="D69" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E69">
         <v>2.3679999999999999</v>
@@ -5418,7 +5418,7 @@
     </row>
     <row r="70" spans="1:16">
       <c r="A70" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B70" t="s">
         <v>15</v>
@@ -5427,7 +5427,7 @@
         <v>221</v>
       </c>
       <c r="D70" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E70">
         <v>2.14</v>
@@ -5468,7 +5468,7 @@
     </row>
     <row r="71" spans="1:16">
       <c r="A71" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B71" t="s">
         <v>0</v>
@@ -5477,7 +5477,7 @@
         <v>225</v>
       </c>
       <c r="D71" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E71">
         <v>2.4969999999999999</v>
@@ -5518,16 +5518,16 @@
     </row>
     <row r="72" spans="1:16">
       <c r="A72" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B72" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C72">
         <v>164</v>
       </c>
       <c r="D72" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E72">
         <v>2.3220000000000001</v>
@@ -5568,7 +5568,7 @@
     </row>
     <row r="73" spans="1:16">
       <c r="A73" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B73" t="s">
         <v>0</v>
@@ -5577,7 +5577,7 @@
         <v>225</v>
       </c>
       <c r="D73" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E73">
         <v>2.5720000000000001</v>
@@ -5618,16 +5618,16 @@
     </row>
     <row r="74" spans="1:16">
       <c r="A74" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B74" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C74">
         <v>206</v>
       </c>
       <c r="D74" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E74">
         <v>2.34</v>
@@ -5668,7 +5668,7 @@
     </row>
     <row r="75" spans="1:16">
       <c r="A75" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B75" t="s">
         <v>0</v>
@@ -5677,7 +5677,7 @@
         <v>225</v>
       </c>
       <c r="D75" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E75">
         <v>2.4390000000000001</v>
@@ -5718,16 +5718,16 @@
     </row>
     <row r="76" spans="1:16">
       <c r="A76" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B76" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C76">
         <v>206</v>
       </c>
       <c r="D76" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E76">
         <v>2.2490000000000001</v>
@@ -5768,7 +5768,7 @@
     </row>
     <row r="77" spans="1:16">
       <c r="A77" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B77" t="s">
         <v>15</v>
@@ -5777,7 +5777,7 @@
         <v>221</v>
       </c>
       <c r="D77" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E77">
         <v>2.1629999999999998</v>

</xml_diff>